<commit_message>
SHLD1 Update - Nordic Platform Operation
Added SHLD1 Code update for Nordic nRF51-DK.  See ...platform
guides\nordic...
</commit_message>
<xml_diff>
--- a/HW Source Files/SENSORSHLD1-EVK-101 HW Design Files/Schematic_BOM/ROHM_SENSORSHLD1-EVK-101_BOM_REV01_2016-03-16.xlsx
+++ b/HW Source Files/SENSORSHLD1-EVK-101 HW Design Files/Schematic_BOM/ROHM_SENSORSHLD1-EVK-101_BOM_REV01_2016-03-16.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="SENSORKIT-MULTISENSORSHIELD" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="176">
   <si>
     <t>Item</t>
   </si>
@@ -489,18 +489,12 @@
     <t>Standard Pitch Through-Hole Female</t>
   </si>
   <si>
-    <t>Last manufacturer should have many of these leftover as I ordered way too many for the last build…  Need to Confirm Before ordering again!</t>
-  </si>
-  <si>
     <t>Header Purchase Info (This is the sum of headers for lines 30-33)</t>
   </si>
   <si>
     <t>32-Pin Header</t>
   </si>
   <si>
-    <t>See Item 35</t>
-  </si>
-  <si>
     <t>CONN HEADER VERT SGL 8POS - Long side on bottom</t>
   </si>
   <si>
@@ -538,12 +532,27 @@
   </si>
   <si>
     <t>KXG03-1034</t>
+  </si>
+  <si>
+    <t>S1012EC-32-ND</t>
+  </si>
+  <si>
+    <t>Break these into line items 29 to 32</t>
+  </si>
+  <si>
+    <t>See Item 34</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>PREC032SAAN-RC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1902,11 +1911,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1927,7 +1937,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -1983,7 +1993,7 @@
         <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -2255,7 +2265,7 @@
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -2507,7 +2517,7 @@
         <v>86</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>142</v>
@@ -2609,7 +2619,7 @@
         <v>97</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>95</v>
@@ -2643,10 +2653,10 @@
         <v>100</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>47</v>
@@ -2711,7 +2721,7 @@
         <v>108</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>149</v>
@@ -2736,7 +2746,7 @@
         <v>137</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>107</v>
@@ -2745,16 +2755,16 @@
         <v>108</v>
       </c>
       <c r="G27" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="H27" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>47</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="7"/>
@@ -2878,7 +2888,7 @@
         <v>49</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -2910,7 +2920,7 @@
         <v>154</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -2942,7 +2952,7 @@
         <v>60</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -2974,19 +2984,19 @@
         <v>54</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G34" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="H34" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J34" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="K34" s="10"/>
       <c r="L34" s="8" t="s">
@@ -3010,19 +3020,19 @@
         <v>52</v>
       </c>
       <c r="F35" s="11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G35" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="H35" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="K35" s="10"/>
       <c r="L35" s="8" t="s">
@@ -3046,19 +3056,19 @@
         <v>54</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="H36" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="K36" s="10"/>
       <c r="L36" s="8" t="s">
@@ -3082,19 +3092,19 @@
         <v>58</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="H37" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>17</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="K37" s="10"/>
       <c r="L37" s="8" t="s">
@@ -3118,7 +3128,7 @@
         <v>58</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
@@ -3141,10 +3151,10 @@
         <v>1</v>
       </c>
       <c r="C39" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D39" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="E39" s="13" t="s">
         <v>110</v>
@@ -3153,13 +3163,21 @@
         <v>111</v>
       </c>
       <c r="G39" s="15" t="s">
-        <v>156</v>
-      </c>
-      <c r="H39" s="15"/>
-      <c r="I39" s="15"/>
-      <c r="J39" s="15"/>
+        <v>174</v>
+      </c>
+      <c r="H39" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="15" t="s">
+        <v>171</v>
+      </c>
       <c r="K39" s="5"/>
-      <c r="L39" s="14"/>
+      <c r="L39" s="14" t="s">
+        <v>172</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3168,7 +3186,7 @@
     <hyperlink ref="J29" r:id="rId3" display="http://www.digikey.com/product-detail/en/NVT2003DP,118/568-8383-2-ND/2763882"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId4"/>
+  <pageSetup scale="41" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId4"/>
   <tableParts count="1">
     <tablePart r:id="rId5"/>
   </tableParts>

</xml_diff>